<commit_message>
[fubo.ding] #96 feature: update template style
</commit_message>
<xml_diff>
--- a/src/main/resources/static/requisition/TR_pt.xlsx
+++ b/src/main/resources/static/requisition/TR_pt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fubo.ding/projects_siglus_to14/siglus-api/src/main/resources/static/requisition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4D3D2F-FB2A-4142-8E10-ED023F277B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98284D1B-B440-F741-B06A-B34386A12123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36440" yWindow="-820" windowWidth="34560" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TR" sheetId="1" r:id="rId1"/>
@@ -615,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -706,9 +706,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -721,6 +718,9 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -777,9 +777,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1208,14 +1205,14 @@
   <dimension ref="A1:AA29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="140" zoomScaleSheetLayoutView="134" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="3.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.59765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.3984375" style="1" customWidth="1"/>
@@ -1354,9 +1351,9 @@
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
       <c r="I5" s="44"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
@@ -1390,14 +1387,14 @@
       <c r="O6" s="15"/>
       <c r="P6" s="15"/>
     </row>
-    <row r="7" spans="1:27" ht="25" customHeight="1">
-      <c r="A7" s="54" t="s">
+    <row r="7" spans="1:27" ht="38" customHeight="1">
+      <c r="A7" s="34" t="s">
         <v>85</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="10" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="13" t="s">
@@ -1434,7 +1431,7 @@
       <c r="I8"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
-      <c r="L8" s="32"/>
+      <c r="L8" s="31"/>
       <c r="M8" s="16"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
@@ -1725,7 +1722,7 @@
       <c r="Z14" s="13"/>
       <c r="AA14" s="13"/>
     </row>
-    <row r="15" spans="1:27" ht="18.25" customHeight="1">
+    <row r="15" spans="1:27" ht="26" customHeight="1">
       <c r="A15" s="29"/>
       <c r="B15" s="24" t="s">
         <v>5</v>
@@ -1974,7 +1971,7 @@
       <c r="AA22" s="13"/>
     </row>
     <row r="23" spans="1:27">
-      <c r="B23" s="33"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
@@ -2049,7 +2046,7 @@
       <c r="L25" s="16"/>
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
-      <c r="O25" s="34"/>
+      <c r="O25" s="33"/>
       <c r="P25" s="19"/>
     </row>
     <row r="26" spans="1:27" ht="30.5" customHeight="1">

</xml_diff>